<commit_message>
akhir dari projek pkl yang melelahkan boy... wuuhuuuuu
</commit_message>
<xml_diff>
--- a/data-siswa.xlsx
+++ b/data-siswa.xlsx
@@ -23,28 +23,28 @@
     <t>SISWA</t>
   </si>
   <si>
-    <t>151080200221</t>
-  </si>
-  <si>
-    <t>FATMALA SARI</t>
-  </si>
-  <si>
-    <t>151080200222</t>
-  </si>
-  <si>
-    <t>INDRA RANDI</t>
-  </si>
-  <si>
-    <t>151080200223</t>
-  </si>
-  <si>
-    <t>AGUNG HERIYANTO</t>
+    <t>1510800200225</t>
+  </si>
+  <si>
+    <t>APRILIA KUSUMA NINGRUM</t>
+  </si>
+  <si>
+    <t>151080200212</t>
+  </si>
+  <si>
+    <t>AHBABUL MUSTHOFA</t>
   </si>
   <si>
     <t>151080200224</t>
   </si>
   <si>
-    <t>LIST INFORMATIKA</t>
+    <t>M.AGUNG HERIYANTO</t>
+  </si>
+  <si>
+    <t>191080200223</t>
+  </si>
+  <si>
+    <t>M.AUNUR ROSIDIN</t>
   </si>
 </sst>
 </file>

</xml_diff>